<commit_message>
se ajusta clase MerchandiseEntryAction, para q tome de forma automatica el punto de venta
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963C17C9-678A-4E95-9958-C408275BA4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D17F03-84FC-4822-A6EC-48F8BCF471F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="2085" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>MSIDN</t>
   </si>
   <si>
-    <t>SERIAL</t>
-  </si>
-  <si>
-    <t>PLU</t>
-  </si>
-  <si>
     <t>URL EPOS</t>
   </si>
   <si>
@@ -114,12 +108,6 @@
     <t>MSI</t>
   </si>
   <si>
-    <t>8957732111198172291</t>
-  </si>
-  <si>
-    <t>8957732111198172290</t>
-  </si>
-  <si>
     <t>3016875982</t>
   </si>
   <si>
@@ -130,6 +118,18 @@
   </si>
   <si>
     <t>732111198172290</t>
+  </si>
+  <si>
+    <t>Vendedor</t>
+  </si>
+  <si>
+    <t>Cedula Cliente</t>
+  </si>
+  <si>
+    <t>10960370</t>
+  </si>
+  <si>
+    <t>667299000</t>
   </si>
 </sst>
 </file>
@@ -188,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -205,6 +205,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -520,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -538,106 +542,106 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -650,45 +654,59 @@
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>1</v>
+      <c r="A10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1">
-        <v>3003324</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1">
-        <v>3003324</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modifican archivos Inventario.csv y Mercanncia.csv
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -122,16 +122,16 @@
     <t>828959809</t>
   </si>
   <si>
-    <t>3016877411</t>
-  </si>
-  <si>
     <t>3016876876</t>
   </si>
   <si>
-    <t>732111198172294</t>
-  </si>
-  <si>
     <t>732111198172293</t>
+  </si>
+  <si>
+    <t>3016875982</t>
+  </si>
+  <si>
+    <t>732111198172291</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -677,10 +677,10 @@
         <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -691,10 +691,10 @@
         <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se realizan ajustes en el assert
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PrepaidAutomation\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EE003E-B525-48E1-8CD2-021B9076B7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>MSIDN</t>
   </si>
@@ -107,6 +108,18 @@
     <t>MSI</t>
   </si>
   <si>
+    <t>3016875982</t>
+  </si>
+  <si>
+    <t>3016875893</t>
+  </si>
+  <si>
+    <t>732111198172291</t>
+  </si>
+  <si>
+    <t>732111198172290</t>
+  </si>
+  <si>
     <t>Vendedor</t>
   </si>
   <si>
@@ -116,28 +129,13 @@
     <t>10960370</t>
   </si>
   <si>
-    <t>12669894</t>
-  </si>
-  <si>
-    <t>828959809</t>
-  </si>
-  <si>
-    <t>3016876876</t>
-  </si>
-  <si>
-    <t>732111198172293</t>
-  </si>
-  <si>
-    <t>3016875982</t>
-  </si>
-  <si>
-    <t>732111198172291</t>
+    <t>667299000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -525,21 +523,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -657,10 +655,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
@@ -671,38 +669,52 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
se realiza ajuste al windex, se crea variable publica Sheet en la clase ReadFileXLSXActions y se ajustan tiempos de la clase Windex.
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,48 +1,187 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EE003E-B525-48E1-8CD2-021B9076B7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4898387C-29EC-4793-AF41-81F55B9D909F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Semilla 2" sheetId="3" r:id="rId1"/>
+    <sheet name="Semilla 3" sheetId="4" r:id="rId2"/>
+    <sheet name="Semilla 4" sheetId="1" r:id="rId3"/>
+    <sheet name="Semilla 5" sheetId="2" r:id="rId4"/>
+    <sheet name="Semilla 6" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="69">
+  <si>
+    <t>URL EPOS</t>
+  </si>
+  <si>
+    <t>URL CRM</t>
+  </si>
+  <si>
+    <t>URL CONFIRMADOR</t>
+  </si>
+  <si>
+    <t>URL GATEWAYCBS</t>
+  </si>
+  <si>
+    <t>URL GATEWAY MG</t>
+  </si>
+  <si>
+    <t>http://10.69.60.57:8180/tigo-pos-web/</t>
+  </si>
+  <si>
+    <t>http://10.69.60.61:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
+  </si>
+  <si>
+    <t>http://10.69.60.57:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>http://10.65.45.12:9001/gatewaycbs/BcServicesInt</t>
+  </si>
+  <si>
+    <t>http://10.65.45.12:9001/gatewaymgint/GatewayMGWSInt</t>
+  </si>
+  <si>
+    <t>URL DB</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>10.69.60.63</t>
+  </si>
+  <si>
+    <t>dev11g</t>
+  </si>
+  <si>
+    <t>ACTIVATOR</t>
+  </si>
+  <si>
+    <t>10.69.60.62</t>
+  </si>
+  <si>
+    <t>desepos</t>
+  </si>
+  <si>
+    <t>epos</t>
+  </si>
+  <si>
+    <t>dev10g</t>
+  </si>
+  <si>
+    <t>postsale</t>
+  </si>
+  <si>
+    <t>10.65.32.74</t>
+  </si>
+  <si>
+    <t>SIEBEL02</t>
+  </si>
+  <si>
+    <t>siebel</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>SN53047304</t>
+  </si>
+  <si>
+    <t>Tigo.2020*</t>
+  </si>
+  <si>
+    <t>Vendedor</t>
+  </si>
+  <si>
+    <t>Cedula Cliente</t>
+  </si>
   <si>
     <t>MSIDN</t>
   </si>
   <si>
-    <t>URL EPOS</t>
-  </si>
-  <si>
-    <t>URL CRM</t>
-  </si>
-  <si>
-    <t>URL CONFIRMADOR</t>
-  </si>
-  <si>
-    <t>URL GATEWAYCBS</t>
-  </si>
-  <si>
-    <t>URL GATEWAY MG</t>
+    <t>MSI</t>
+  </si>
+  <si>
+    <t>10960370</t>
+  </si>
+  <si>
+    <t>984108505</t>
+  </si>
+  <si>
+    <t>3016875982</t>
+  </si>
+  <si>
+    <t>732111198172291</t>
+  </si>
+  <si>
+    <t>835244140</t>
+  </si>
+  <si>
+    <t>3016875893</t>
+  </si>
+  <si>
+    <t>732111198172290</t>
+  </si>
+  <si>
+    <t>667299000</t>
+  </si>
+  <si>
+    <t>http://10.69.60.224:8180/tigo-pos-web/</t>
+  </si>
+  <si>
+    <t>http://10.69.60.149:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
+  </si>
+  <si>
+    <t>http://10.69.60.224:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>10.69.60.103</t>
+  </si>
+  <si>
+    <t>DEV11G</t>
+  </si>
+  <si>
+    <t>10.69.60.102</t>
+  </si>
+  <si>
+    <t>10.65.32.76</t>
   </si>
   <si>
     <t>http://10.69.60.77:8180/tigo-pos-web/</t>
@@ -54,89 +193,65 @@
     <t>http://10.69.60.77:8180/tigo-pos-web/wap/windex.wml</t>
   </si>
   <si>
-    <t>http://10.65.45.12:9001/gatewaycbs/BcServicesInt</t>
-  </si>
-  <si>
-    <t>URL DB</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>10.69.60.89</t>
   </si>
   <si>
-    <t>DEV11G</t>
-  </si>
-  <si>
-    <t>ACTIVATOR</t>
-  </si>
-  <si>
     <t>10.69.60.88</t>
   </si>
   <si>
-    <t>desepos</t>
-  </si>
-  <si>
-    <t>epos</t>
-  </si>
-  <si>
-    <t>dev10g</t>
-  </si>
-  <si>
-    <t>postsale</t>
-  </si>
-  <si>
-    <t>10.65.32.74</t>
-  </si>
-  <si>
     <t>siebel04</t>
   </si>
   <si>
-    <t>siebel</t>
-  </si>
-  <si>
-    <t>service</t>
-  </si>
-  <si>
-    <t>http://10.65.45.12:9001/gatewaymgint/GatewayMGWSInt</t>
-  </si>
-  <si>
-    <t>MSI</t>
-  </si>
-  <si>
-    <t>3016875982</t>
-  </si>
-  <si>
-    <t>3016875893</t>
-  </si>
-  <si>
-    <t>732111198172291</t>
-  </si>
-  <si>
-    <t>732111198172290</t>
-  </si>
-  <si>
-    <t>Vendedor</t>
-  </si>
-  <si>
-    <t>Cedula Cliente</t>
-  </si>
-  <si>
-    <t>10960370</t>
-  </si>
-  <si>
-    <t>667299000</t>
+    <t>http://10.69.60.97:8180/tigo-pos-web/</t>
+  </si>
+  <si>
+    <t>http://10.69.60.98:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
+  </si>
+  <si>
+    <t>http://10.69.60.97:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>10.69.60.94</t>
+  </si>
+  <si>
+    <t>10.69.60.93</t>
+  </si>
+  <si>
+    <t>DESEPOS</t>
+  </si>
+  <si>
+    <t>EPOS</t>
+  </si>
+  <si>
+    <t>DEV10G</t>
+  </si>
+  <si>
+    <t>SIEBEL</t>
+  </si>
+  <si>
+    <t>http://10.69.60.75:8180/tigo-pos-web/</t>
+  </si>
+  <si>
+    <t>http://10.69.60.84:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
+  </si>
+  <si>
+    <t>http://10.69.60.75:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>10.69.60.87</t>
+  </si>
+  <si>
+    <t>10.69.60.86</t>
+  </si>
+  <si>
+    <t>SIEBEL03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +281,34 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF242424"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -204,11 +347,16 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -524,10 +672,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1">
+      <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1">
+      <c r="A9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="7"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1">
+      <c r="A8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="F14" s="7"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -542,36 +1103,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -579,144 +1140,540 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="6"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="9" customFormat="1">
+      <c r="A8" s="8"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="7"/>
+    <row r="9" spans="1:5" s="9" customFormat="1">
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="D10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>34</v>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>34</v>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1">
+      <c r="A8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="D14" s="7"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="A8:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1">
+      <c r="A8" s="6"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1">
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se modifican ControlActivationActions para boton confirmar
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PrepaidAutomation\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4898387C-29EC-4793-AF41-81F55B9D909F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 2" sheetId="3" r:id="rId1"/>
-    <sheet name="Semilla 3" sheetId="4" r:id="rId2"/>
+    <sheet name="Semilla 13" sheetId="4" r:id="rId2"/>
     <sheet name="Semilla 4" sheetId="1" r:id="rId3"/>
     <sheet name="Semilla 5" sheetId="2" r:id="rId4"/>
     <sheet name="Semilla 6" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="70">
   <si>
     <t>URL EPOS</t>
   </si>
@@ -172,15 +171,9 @@
     <t>http://10.69.60.224:8180/tigo-pos-web/wap/windex.wml</t>
   </si>
   <si>
-    <t>10.69.60.103</t>
-  </si>
-  <si>
     <t>DEV11G</t>
   </si>
   <si>
-    <t>10.69.60.102</t>
-  </si>
-  <si>
     <t>10.65.32.76</t>
   </si>
   <si>
@@ -245,12 +238,21 @@
   </si>
   <si>
     <t>SIEBEL03</t>
+  </si>
+  <si>
+    <t>10.69.60.227</t>
+  </si>
+  <si>
+    <t>10.69.60.223</t>
+  </si>
+  <si>
+    <t>SIEBCBS1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -671,20 +673,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="34.81640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="4" max="4" width="25.7265625" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
@@ -872,31 +874,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="5" max="5" width="36.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
@@ -949,10 +951,10 @@
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>16</v>
@@ -963,10 +965,10 @@
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -977,7 +979,7 @@
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>20</v>
@@ -991,10 +993,10 @@
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -1072,11 +1074,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -1084,21 +1086,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1120,13 +1122,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -1151,10 +1153,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>16</v>
@@ -1165,7 +1167,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
@@ -1179,7 +1181,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>20</v>
@@ -1196,7 +1198,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -1271,10 +1273,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1282,20 +1284,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
@@ -1317,13 +1319,13 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -1348,10 +1350,10 @@
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>16</v>
@@ -1362,24 +1364,24 @@
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>21</v>
@@ -1390,10 +1392,10 @@
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -1471,29 +1473,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="A8:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
@@ -1517,13 +1519,13 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -1548,7 +1550,7 @@
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>15</v>
@@ -1562,10 +1564,10 @@
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1576,7 +1578,7 @@
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>20</v>
@@ -1593,7 +1595,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -1668,11 +1670,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se realiza creacion de scenario semilla 4, se ajustan metodos para que reciban la hoja de excel donde se encuentra la data para la prueba.
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8014132-3326-425F-9918-9AA6AFB83280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA56CB3-9E44-4B6D-A345-A54DF9E07311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 2" sheetId="3" r:id="rId1"/>
-    <sheet name="Semilla 3" sheetId="4" r:id="rId2"/>
+    <sheet name="Semilla 13" sheetId="4" r:id="rId2"/>
     <sheet name="Semilla 4" sheetId="1" r:id="rId3"/>
     <sheet name="Semilla 5" sheetId="2" r:id="rId4"/>
     <sheet name="Semilla 6" sheetId="5" r:id="rId5"/>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="66">
   <si>
     <t>URL EPOS</t>
   </si>
@@ -115,18 +116,6 @@
     <t>siebel</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>SN53047304</t>
-  </si>
-  <si>
-    <t>Tigo.2020*</t>
-  </si>
-  <si>
     <t>Vendedor</t>
   </si>
   <si>
@@ -172,58 +161,61 @@
     <t>http://10.69.60.224:8180/tigo-pos-web/wap/windex.wml</t>
   </si>
   <si>
-    <t>10.69.60.103</t>
+    <t>10.69.60.227</t>
   </si>
   <si>
     <t>DEV11G</t>
   </si>
   <si>
-    <t>10.69.60.102</t>
+    <t>10.69.60.223</t>
+  </si>
+  <si>
+    <t>DESEPOS</t>
+  </si>
+  <si>
+    <t>SIEBCBS1</t>
+  </si>
+  <si>
+    <t>http://10.69.60.77:8180/tigo-pos-web/</t>
+  </si>
+  <si>
+    <t>http://10.69.60.85:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
+  </si>
+  <si>
+    <t>http://10.69.60.77:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>10.69.60.89</t>
+  </si>
+  <si>
+    <t>10.69.60.88</t>
+  </si>
+  <si>
+    <t>siebel04</t>
+  </si>
+  <si>
+    <t>http://10.69.60.97:8180/tigo-pos-web/</t>
+  </si>
+  <si>
+    <t>http://10.69.60.98:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
+  </si>
+  <si>
+    <t>http://10.69.60.97:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>10.69.60.94</t>
+  </si>
+  <si>
+    <t>10.69.60.93</t>
+  </si>
+  <si>
+    <t>EPOS</t>
+  </si>
+  <si>
+    <t>DEV10G</t>
   </si>
   <si>
     <t>10.65.32.76</t>
-  </si>
-  <si>
-    <t>http://10.69.60.77:8180/tigo-pos-web/</t>
-  </si>
-  <si>
-    <t>http://10.69.60.85:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
-  </si>
-  <si>
-    <t>http://10.69.60.77:8180/tigo-pos-web/wap/windex.wml</t>
-  </si>
-  <si>
-    <t>10.69.60.89</t>
-  </si>
-  <si>
-    <t>10.69.60.88</t>
-  </si>
-  <si>
-    <t>siebel04</t>
-  </si>
-  <si>
-    <t>http://10.69.60.97:8180/tigo-pos-web/</t>
-  </si>
-  <si>
-    <t>http://10.69.60.98:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
-  </si>
-  <si>
-    <t>http://10.69.60.97:8180/tigo-pos-web/wap/windex.wml</t>
-  </si>
-  <si>
-    <t>10.69.60.94</t>
-  </si>
-  <si>
-    <t>10.69.60.93</t>
-  </si>
-  <si>
-    <t>DESEPOS</t>
-  </si>
-  <si>
-    <t>EPOS</t>
-  </si>
-  <si>
-    <t>DEV10G</t>
   </si>
   <si>
     <t>SIEBEL</t>
@@ -251,7 +243,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,26 +281,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF242424"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -331,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -344,20 +316,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -673,20 +632,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="13"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
@@ -794,80 +752,69 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1">
-      <c r="A9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1">
-      <c r="A13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -878,15 +825,16 @@
     <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -917,13 +865,13 @@
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -948,10 +896,10 @@
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>16</v>
@@ -962,10 +910,10 @@
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -976,7 +924,7 @@
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>20</v>
@@ -990,10 +938,10 @@
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -1003,71 +951,63 @@
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1">
-      <c r="A8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1">
-      <c r="D9" s="4"/>
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="1" customFormat="1">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="1" customFormat="1">
-      <c r="A13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="F14" s="7"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="F12" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1084,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1119,13 +1059,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -1150,10 +1090,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>16</v>
@@ -1164,7 +1104,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
@@ -1178,7 +1118,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>20</v>
@@ -1195,7 +1135,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -1204,68 +1144,60 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="9" customFormat="1">
-      <c r="A8" s="8"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" s="9" customFormat="1">
-      <c r="D9" s="4"/>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1282,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1316,13 +1248,13 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -1347,10 +1279,10 @@
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>16</v>
@@ -1361,24 +1293,24 @@
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>21</v>
@@ -1389,10 +1321,10 @@
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -1402,71 +1334,63 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1">
-      <c r="A8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1">
-      <c r="D9" s="4"/>
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1">
-      <c r="A13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="D14" s="7"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="D12" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1482,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="A8:XFD9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1516,13 +1440,13 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -1547,7 +1471,7 @@
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>15</v>
@@ -1561,10 +1485,10 @@
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1575,7 +1499,7 @@
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>20</v>
@@ -1592,7 +1516,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -1602,67 +1526,59 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1">
-      <c r="A8" s="6"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1">
-      <c r="D9" s="10"/>
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1">
-      <c r="A13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se realizan cambios para sanity en semilla 4, logueandose desde los gets
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PrepaidAutomation\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5951DE-069F-4589-A58A-E68B7EB1CE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 2" sheetId="3" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Semilla 5" sheetId="2" r:id="rId4"/>
     <sheet name="Semilla 6" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="72">
   <si>
     <t>URL EPOS</t>
   </si>
@@ -237,12 +236,30 @@
   </si>
   <si>
     <t>SIEBEL03</t>
+  </si>
+  <si>
+    <t>CQ10960370</t>
+  </si>
+  <si>
+    <t>Tigo.2022*</t>
+  </si>
+  <si>
+    <t>rutaWinWap</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\Winwap Technologies\WinWAP for Windows 4.2\WinWAP4.exe</t>
+  </si>
+  <si>
+    <t>SN53047304</t>
+  </si>
+  <si>
+    <t>Tigo.2020*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -274,12 +291,11 @@
       <family val="3"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF297BDE"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -316,7 +332,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -631,23 +649,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="34.81640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="4" max="4" width="25.7265625" customWidth="1"/>
+    <col min="5" max="5" width="49.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -663,8 +681,17 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -680,8 +707,17 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1">
+      <c r="F2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -695,7 +731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1">
+    <row r="4" spans="1:8" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -709,7 +745,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1">
+    <row r="5" spans="1:8" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -723,7 +759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1">
+    <row r="6" spans="1:8" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -737,7 +773,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1">
+    <row r="7" spans="1:8" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -751,7 +787,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1">
+    <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -765,7 +801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1">
+    <row r="9" spans="1:8" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -779,7 +815,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1">
+    <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -793,7 +829,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1">
+    <row r="11" spans="1:8" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -807,22 +843,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="B16" s="6"/>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="C19" s="6"/>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="6"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -830,23 +857,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="5" max="5" width="49.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -862,8 +889,17 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -879,8 +915,17 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1">
+      <c r="F2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -894,7 +939,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1">
+    <row r="4" spans="1:8" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>40</v>
       </c>
@@ -908,7 +953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1">
+    <row r="5" spans="1:8" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
@@ -922,7 +967,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1">
+    <row r="6" spans="1:8" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
@@ -936,7 +981,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1">
+    <row r="7" spans="1:8" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -950,7 +995,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1">
+    <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -964,7 +1009,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1">
+    <row r="9" spans="1:8" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -978,7 +1023,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1">
+    <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -992,7 +1037,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1">
+    <row r="11" spans="1:8" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1008,11 +1053,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -1020,24 +1065,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1053,8 +1098,17 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1070,8 +1124,17 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1085,7 +1148,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
         <v>48</v>
       </c>
@@ -1099,7 +1162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
         <v>49</v>
       </c>
@@ -1113,7 +1176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -1127,7 +1190,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -1141,7 +1204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1155,7 +1218,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1169,7 +1232,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1183,7 +1246,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1199,11 +1262,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{073D1BD7-782F-4154-8E2B-5F400B16F56E}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -1211,23 +1274,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1243,8 +1306,17 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
@@ -1260,8 +1332,17 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1">
+      <c r="F2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1275,7 +1356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1">
+    <row r="4" spans="1:8" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>54</v>
       </c>
@@ -1289,7 +1370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1">
+    <row r="5" spans="1:8" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
@@ -1303,7 +1384,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1">
+    <row r="6" spans="1:8" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>55</v>
       </c>
@@ -1317,7 +1398,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1">
+    <row r="7" spans="1:8" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>58</v>
       </c>
@@ -1331,7 +1412,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1">
+    <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1345,7 +1426,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1">
+    <row r="9" spans="1:8" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1359,7 +1440,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1">
+    <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1373,7 +1454,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1">
+    <row r="11" spans="1:8" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1389,34 +1470,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1432,8 +1513,17 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>60</v>
       </c>
@@ -1449,8 +1539,17 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1">
+      <c r="F2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1464,7 +1563,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1">
+    <row r="4" spans="1:8" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>63</v>
       </c>
@@ -1478,7 +1577,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1">
+    <row r="5" spans="1:8" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>64</v>
       </c>
@@ -1492,7 +1591,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1">
+    <row r="6" spans="1:8" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
@@ -1506,7 +1605,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1">
+    <row r="7" spans="1:8" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
@@ -1520,7 +1619,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1">
+    <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1534,7 +1633,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1">
+    <row r="9" spans="1:8" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1548,7 +1647,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1">
+    <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1562,7 +1661,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1">
+    <row r="11" spans="1:8" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1578,11 +1677,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>